<commit_message>
In/Output costs in separate input df
</commit_message>
<xml_diff>
--- a/Spine_Projects/01_input_data/01_input_raw/Energy Prices/district_heating_price_cap.xlsx
+++ b/Spine_Projects/01_input_data/01_input_raw/Energy Prices/district_heating_price_cap.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jfg.eco\Documents\GitHub\Nord_H2ub\spine_projects\01_input_data\01_input_raw\energy_prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studentcbs-my.sharepoint.com/personal/djh_eco_cbs_dk/Documents/Documents/GitHub/Nord_H2ub/Spine_Projects/01_input_data/01_input_raw/Energy Prices/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DA13C8-180D-4980-BB9F-AA3F8C9D2A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{94DA13C8-180D-4980-BB9F-AA3F8C9D2A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AD2823F-E044-429E-B816-CD9F230FA418}"/>
   <bookViews>
-    <workbookView xWindow="-5070" yWindow="-21720" windowWidth="38640" windowHeight="21120" xr2:uid="{BDF52CB5-8AF7-4070-9BAF-21BBD77363FF}"/>
+    <workbookView xWindow="6465" yWindow="-20085" windowWidth="33180" windowHeight="16380" xr2:uid="{BDF52CB5-8AF7-4070-9BAF-21BBD77363FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Price_Cap_Calculation" sheetId="1" r:id="rId1"/>
@@ -212,9 +212,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="6">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -317,6 +314,9 @@
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -335,12 +335,12 @@
   <autoFilter ref="A1:G4" xr:uid="{8F68E1AD-1E8B-4ACE-A9DE-2514707D9B42}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{A6FEAB50-FA63-446B-B963-FFE2083525E3}" name="Price cap"/>
-    <tableColumn id="8" xr3:uid="{F08150EC-6285-44C7-B582-FF0BA3697B79}" name="2018" dataDxfId="0">
+    <tableColumn id="8" xr3:uid="{F08150EC-6285-44C7-B582-FF0BA3697B79}" name="2018" dataDxfId="5">
       <calculatedColumnFormula array="1">Table2[2018]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{E77E28C3-6031-4C08-B54D-35A5A0CCC2F3}" name="2019"/>
     <tableColumn id="3" xr3:uid="{9BF1D066-C7E0-4A13-8E0A-07795D412DD6}" name="2020"/>
-    <tableColumn id="4" xr3:uid="{94EEE701-C19A-4405-B469-9A9B9CFF43D5}" name="2021" dataDxfId="5">
+    <tableColumn id="4" xr3:uid="{94EEE701-C19A-4405-B469-9A9B9CFF43D5}" name="2021" dataDxfId="4">
       <calculatedColumnFormula array="1">Table2[2018]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{8EC6DBC7-5CD1-4CC1-B48E-052446EA7F03}" name="2022"/>
@@ -373,16 +373,16 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}" name="Table2" displayName="Table2" ref="A5:G6" totalsRowShown="0" tableBorderDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}" name="Table2" displayName="Table2" ref="A5:G6" totalsRowShown="0" tableBorderDxfId="3">
   <autoFilter ref="A5:G6" xr:uid="{7BF6279C-0A47-4882-8A47-FBB883A7F586}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{D3E85E44-117A-4A3D-B167-80884115B936}" name="Price cap"/>
     <tableColumn id="2" xr3:uid="{9FB8A1A3-5B94-42D9-8374-F609ECDC4806}" name="2018"/>
     <tableColumn id="3" xr3:uid="{BC877BDF-034D-4BAE-8945-44CE9F9FA3BF}" name="2019"/>
     <tableColumn id="4" xr3:uid="{C3208B9F-5220-4737-97F7-04B4B458599B}" name="2020"/>
-    <tableColumn id="5" xr3:uid="{717424EF-4D50-42EC-ABE0-707DA0FB5BFE}" name="2021" dataDxfId="3"/>
-    <tableColumn id="6" xr3:uid="{7B8608B1-3E6A-44D6-B820-4DE5304A1F9D}" name="2022" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{B8C7C939-753F-4966-977C-1E33CD2C3DDD}" name="2023" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{717424EF-4D50-42EC-ABE0-707DA0FB5BFE}" name="2021" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7B8608B1-3E6A-44D6-B820-4DE5304A1F9D}" name="2022" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{B8C7C939-753F-4966-977C-1E33CD2C3DDD}" name="2023" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -708,7 +708,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -844,7 +844,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>